<commit_message>
adicionado nova versão dos slides
</commit_message>
<xml_diff>
--- a/doc/pfc/resultados/teste_gerador_rotas/5_GPS+Retorno/analise_erro/analise_erro.xlsx
+++ b/doc/pfc/resultados/teste_gerador_rotas/5_GPS+Retorno/analise_erro/analise_erro.xlsx
@@ -14,23 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Pontos</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Comandado</t>
   </si>
   <si>
@@ -50,6 +38,15 @@
   </si>
   <si>
     <t>Distância Y (m)</t>
+  </si>
+  <si>
+    <t>Latitude (º)</t>
+  </si>
+  <si>
+    <t>Longitude (º)</t>
+  </si>
+  <si>
+    <t>Altura (m)</t>
   </si>
 </sst>
 </file>
@@ -58,8 +55,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00000000"/>
-    <numFmt numFmtId="172" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -225,62 +222,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -290,6 +275,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,12 +596,12 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G7" sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
@@ -617,236 +615,237 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="9"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="19">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <v>-27.605003865499999</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>-48.519523063999998</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>2.2999999523199999</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>0.68197244650199995</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>0.10856352374</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="6">
         <v>0.28574701249000001</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="20">
         <v>2</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="4">
         <v>-27.605023376799998</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>-48.519509189899999</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>2.2999999523199999</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>0.407119563781</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>0.48060256987799999</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="6">
         <v>0.28524088655000002</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="20">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>-27.605050960300002</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>-48.519517590600003</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>2.2000000476800001</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>0.10874076141</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>0.73232934810200001</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="6">
         <v>0.18458923717</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="19">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>-27.605035730899999</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>-48.519580118199997</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>2.7999999523199999</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>0.32173895742699998</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>0.364112664014</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="6">
         <v>0.78553023506999997</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+      <c r="A7" s="21">
         <v>5</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="9">
         <v>-27.604992714000002</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="9">
         <v>-48.519565049100002</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="10">
         <v>2.5999999046300002</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="10">
         <v>0.113740563276</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="10">
         <v>0.65223406069000001</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="11">
         <v>0.58434612576</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>-27.605003009800001</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="2">
         <v>-48.519529990599999</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <v>2.01425293983</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
+      <c r="B14" s="2">
         <v>-27.605019115800001</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="2">
         <v>-48.519513409399998</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="3">
         <v>2.0147590657699999</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
+      <c r="B15" s="2">
         <v>-27.605044335500001</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="2">
         <v>-48.519516638500001</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="3">
         <v>2.0154108105100002</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
+      <c r="B16" s="2">
         <v>-27.6050389567</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="2">
         <v>-48.519576786800002</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="3">
         <v>2.0144697172499999</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="14">
+      <c r="B17" s="7">
         <v>-27.604998617300001</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="7">
         <v>-48.519566068099998</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="8">
         <v>2.01565377887</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>